<commit_message>
fix typo and show gridlines
</commit_message>
<xml_diff>
--- a/Checklists/Mobile_App_Security_Checklist-French_1.1.3.1.xlsx
+++ b/Checklists/Mobile_App_Security_Checklist-French_1.1.3.1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\owasp-mstg\owasp-mstg-20200426-2049.work\Checklists\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\owasp-mstg\checklist.work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220286EC-2DD2-4BFB-984B-26CB3DCC6C94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F13E044C-1CA2-448F-AAEF-83333E971EFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="200" windowWidth="18840" windowHeight="9920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="420" yWindow="280" windowWidth="18780" windowHeight="9920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau de Bord" sheetId="6" r:id="rId1"/>
@@ -2763,32 +2763,74 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2807,47 +2849,42 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2858,33 +2895,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2896,16 +2906,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="12" borderId="22" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -4208,48 +4208,48 @@
   <sheetData>
     <row r="1" spans="2:4" ht="8.15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="153" t="s">
+      <c r="B2" s="141" t="s">
         <v>209</v>
       </c>
-      <c r="C2" s="154"/>
-      <c r="D2" s="155"/>
+      <c r="C2" s="142"/>
+      <c r="D2" s="143"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="156"/>
-      <c r="C3" s="157"/>
-      <c r="D3" s="158"/>
+      <c r="B3" s="144"/>
+      <c r="C3" s="145"/>
+      <c r="D3" s="146"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B4" s="156"/>
-      <c r="C4" s="157"/>
-      <c r="D4" s="158"/>
+      <c r="B4" s="144"/>
+      <c r="C4" s="145"/>
+      <c r="D4" s="146"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="156"/>
-      <c r="C5" s="157"/>
-      <c r="D5" s="158"/>
+      <c r="B5" s="144"/>
+      <c r="C5" s="145"/>
+      <c r="D5" s="146"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B6" s="156"/>
-      <c r="C6" s="157"/>
-      <c r="D6" s="158"/>
+      <c r="B6" s="144"/>
+      <c r="C6" s="145"/>
+      <c r="D6" s="146"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="156"/>
-      <c r="C7" s="157"/>
-      <c r="D7" s="158"/>
+      <c r="B7" s="144"/>
+      <c r="C7" s="145"/>
+      <c r="D7" s="146"/>
     </row>
     <row r="8" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="159"/>
-      <c r="C8" s="160"/>
-      <c r="D8" s="161"/>
+      <c r="B8" s="147"/>
+      <c r="C8" s="148"/>
+      <c r="D8" s="149"/>
     </row>
     <row r="9" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B9" s="162" t="s">
+      <c r="B9" s="150" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="144"/>
-      <c r="D9" s="145"/>
+      <c r="C9" s="151"/>
+      <c r="D9" s="152"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B10" s="63" t="s">
@@ -4259,29 +4259,29 @@
       <c r="D10" s="65"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B11" s="165" t="s">
+      <c r="B11" s="155" t="s">
         <v>225</v>
       </c>
-      <c r="C11" s="165"/>
+      <c r="C11" s="155"/>
       <c r="D11" s="70">
         <v>1.2</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B12" s="165" t="s">
+      <c r="B12" s="155" t="s">
         <v>273</v>
       </c>
-      <c r="C12" s="165"/>
+      <c r="C12" s="155"/>
       <c r="D12" s="66" t="str">
         <f>HYPERLINK(CONCATENATE("https://github.com/OWASP/owasp-masvs/blob/",VERSION_MASVS,"/Document/"))</f>
         <v>https://github.com/OWASP/owasp-masvs/blob/1.2/Document/</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B13" s="163" t="s">
+      <c r="B13" s="153" t="s">
         <v>271</v>
       </c>
-      <c r="C13" s="164"/>
+      <c r="C13" s="154"/>
       <c r="D13" s="42" t="s">
         <v>362</v>
       </c>
@@ -4318,55 +4318,55 @@
       <c r="D17" s="42"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B18" s="137" t="s">
+      <c r="B18" s="139" t="s">
         <v>196</v>
       </c>
-      <c r="C18" s="152"/>
+      <c r="C18" s="140"/>
       <c r="D18" s="11"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B19" s="142" t="s">
+      <c r="B19" s="137" t="s">
         <v>85</v>
       </c>
-      <c r="C19" s="143"/>
+      <c r="C19" s="138"/>
       <c r="D19" s="11"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B20" s="142" t="s">
+      <c r="B20" s="137" t="s">
         <v>197</v>
       </c>
-      <c r="C20" s="143"/>
+      <c r="C20" s="138"/>
       <c r="D20" s="11"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B21" s="142" t="s">
+      <c r="B21" s="137" t="s">
         <v>86</v>
       </c>
-      <c r="C21" s="143"/>
+      <c r="C21" s="138"/>
       <c r="D21" s="11"/>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="142" t="s">
+      <c r="B22" s="137" t="s">
         <v>198</v>
       </c>
-      <c r="C22" s="143"/>
+      <c r="C22" s="138"/>
       <c r="D22" s="11" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="142" t="s">
+      <c r="B23" s="137" t="s">
         <v>200</v>
       </c>
-      <c r="C23" s="143"/>
+      <c r="C23" s="138"/>
       <c r="D23" s="11" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B24" s="144"/>
-      <c r="C24" s="144"/>
-      <c r="D24" s="145"/>
+      <c r="B24" s="151"/>
+      <c r="C24" s="151"/>
+      <c r="D24" s="152"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
@@ -4383,37 +4383,37 @@
       <c r="D26" s="11"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B27" s="142" t="s">
+      <c r="B27" s="137" t="s">
         <v>204</v>
       </c>
-      <c r="C27" s="143"/>
+      <c r="C27" s="138"/>
       <c r="D27" s="11"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B28" s="142" t="s">
+      <c r="B28" s="137" t="s">
         <v>87</v>
       </c>
-      <c r="C28" s="143"/>
+      <c r="C28" s="138"/>
       <c r="D28" s="11"/>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B29" s="142" t="s">
+      <c r="B29" s="137" t="s">
         <v>64</v>
       </c>
-      <c r="C29" s="143"/>
+      <c r="C29" s="138"/>
       <c r="D29" s="11"/>
     </row>
     <row r="30" spans="2:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="150" t="s">
+      <c r="B30" s="164" t="s">
         <v>235</v>
       </c>
-      <c r="C30" s="151"/>
+      <c r="C30" s="165"/>
       <c r="D30" s="11"/>
     </row>
     <row r="31" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B31" s="146"/>
-      <c r="C31" s="146"/>
-      <c r="D31" s="147"/>
+      <c r="B31" s="160"/>
+      <c r="C31" s="160"/>
+      <c r="D31" s="161"/>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
@@ -4430,37 +4430,37 @@
       <c r="D33" s="11"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B34" s="142" t="s">
+      <c r="B34" s="137" t="s">
         <v>206</v>
       </c>
-      <c r="C34" s="143"/>
+      <c r="C34" s="138"/>
       <c r="D34" s="11"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B35" s="142" t="s">
+      <c r="B35" s="137" t="s">
         <v>87</v>
       </c>
-      <c r="C35" s="143"/>
+      <c r="C35" s="138"/>
       <c r="D35" s="11"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B36" s="142" t="s">
+      <c r="B36" s="137" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="143"/>
+      <c r="C36" s="138"/>
       <c r="D36" s="11"/>
     </row>
     <row r="37" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="148" t="s">
+      <c r="B37" s="162" t="s">
         <v>236</v>
       </c>
-      <c r="C37" s="149"/>
+      <c r="C37" s="163"/>
       <c r="D37" s="11"/>
     </row>
     <row r="38" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B38" s="144"/>
-      <c r="C38" s="144"/>
-      <c r="D38" s="145"/>
+      <c r="B38" s="151"/>
+      <c r="C38" s="151"/>
+      <c r="D38" s="152"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
@@ -4470,97 +4470,97 @@
       <c r="D39" s="3"/>
     </row>
     <row r="40" spans="2:4" ht="15.5" x14ac:dyDescent="0.2">
-      <c r="B40" s="139"/>
-      <c r="C40" s="140"/>
-      <c r="D40" s="141"/>
+      <c r="B40" s="156"/>
+      <c r="C40" s="157"/>
+      <c r="D40" s="158"/>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B41" s="137" t="s">
+      <c r="B41" s="139" t="s">
         <v>107</v>
       </c>
-      <c r="C41" s="138"/>
+      <c r="C41" s="159"/>
       <c r="D41" s="24"/>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B42" s="137" t="s">
+      <c r="B42" s="139" t="s">
         <v>108</v>
       </c>
-      <c r="C42" s="138"/>
+      <c r="C42" s="159"/>
       <c r="D42" s="24"/>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B43" s="137" t="s">
+      <c r="B43" s="139" t="s">
         <v>109</v>
       </c>
-      <c r="C43" s="138"/>
+      <c r="C43" s="159"/>
       <c r="D43" s="24"/>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B44" s="137" t="s">
+      <c r="B44" s="139" t="s">
         <v>208</v>
       </c>
-      <c r="C44" s="138"/>
+      <c r="C44" s="159"/>
       <c r="D44" s="25"/>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B45" s="137" t="s">
+      <c r="B45" s="139" t="s">
         <v>110</v>
       </c>
-      <c r="C45" s="138"/>
+      <c r="C45" s="159"/>
       <c r="D45" s="24"/>
     </row>
     <row r="46" spans="2:4" ht="15.5" x14ac:dyDescent="0.2">
-      <c r="B46" s="139"/>
-      <c r="C46" s="140"/>
-      <c r="D46" s="141"/>
+      <c r="B46" s="156"/>
+      <c r="C46" s="157"/>
+      <c r="D46" s="158"/>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B47" s="137" t="s">
+      <c r="B47" s="139" t="s">
         <v>107</v>
       </c>
-      <c r="C47" s="138"/>
+      <c r="C47" s="159"/>
       <c r="D47" s="24"/>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B48" s="137" t="s">
+      <c r="B48" s="139" t="s">
         <v>108</v>
       </c>
-      <c r="C48" s="138"/>
+      <c r="C48" s="159"/>
       <c r="D48" s="24"/>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B49" s="137" t="s">
+      <c r="B49" s="139" t="s">
         <v>109</v>
       </c>
-      <c r="C49" s="138"/>
+      <c r="C49" s="159"/>
       <c r="D49" s="24"/>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B50" s="137" t="s">
+      <c r="B50" s="139" t="s">
         <v>208</v>
       </c>
-      <c r="C50" s="138"/>
+      <c r="C50" s="159"/>
       <c r="D50" s="25"/>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B51" s="137" t="s">
+      <c r="B51" s="139" t="s">
         <v>110</v>
       </c>
-      <c r="C51" s="138"/>
+      <c r="C51" s="159"/>
       <c r="D51" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B2:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="B47:C47"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="B40:D40"/>
@@ -4575,16 +4575,16 @@
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B2:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <phoneticPr fontId="32"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4630,11 +4630,11 @@
       <c r="F3" s="7"/>
     </row>
     <row r="4" spans="2:24" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B4" s="182"/>
-      <c r="C4" s="182"/>
-      <c r="D4" s="182"/>
-      <c r="E4" s="182"/>
-      <c r="F4" s="182"/>
+      <c r="B4" s="166"/>
+      <c r="C4" s="166"/>
+      <c r="D4" s="166"/>
+      <c r="E4" s="166"/>
+      <c r="F4" s="166"/>
     </row>
     <row r="5" spans="2:24" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="19"/>
@@ -4649,16 +4649,16 @@
       <c r="D6" s="20"/>
       <c r="E6" s="20"/>
       <c r="F6" s="20"/>
-      <c r="G6" s="183" t="s">
+      <c r="G6" s="176" t="s">
         <v>194</v>
       </c>
-      <c r="H6" s="184"/>
-      <c r="I6" s="185"/>
-      <c r="V6" s="166" t="s">
+      <c r="H6" s="177"/>
+      <c r="I6" s="178"/>
+      <c r="V6" s="179" t="s">
         <v>233</v>
       </c>
-      <c r="W6" s="167"/>
-      <c r="X6" s="168"/>
+      <c r="W6" s="180"/>
+      <c r="X6" s="181"/>
     </row>
     <row r="7" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="12"/>
@@ -4673,18 +4673,18 @@
       <c r="D8" s="19"/>
       <c r="E8" s="19"/>
       <c r="F8" s="19"/>
-      <c r="G8" s="169">
+      <c r="G8" s="167">
         <f>AVERAGE(G43:G50)*5</f>
         <v>0</v>
       </c>
-      <c r="H8" s="170"/>
-      <c r="I8" s="171"/>
-      <c r="V8" s="169">
+      <c r="H8" s="168"/>
+      <c r="I8" s="169"/>
+      <c r="V8" s="167">
         <f>AVERAGE(K43:K50)*5</f>
         <v>0</v>
       </c>
-      <c r="W8" s="170"/>
-      <c r="X8" s="171"/>
+      <c r="W8" s="168"/>
+      <c r="X8" s="169"/>
     </row>
     <row r="9" spans="2:24" ht="91" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="20"/>
@@ -4692,12 +4692,12 @@
       <c r="D9" s="20"/>
       <c r="E9" s="20"/>
       <c r="F9" s="20"/>
-      <c r="G9" s="172"/>
-      <c r="H9" s="173"/>
-      <c r="I9" s="174"/>
-      <c r="V9" s="172"/>
-      <c r="W9" s="173"/>
-      <c r="X9" s="174"/>
+      <c r="G9" s="170"/>
+      <c r="H9" s="171"/>
+      <c r="I9" s="172"/>
+      <c r="V9" s="170"/>
+      <c r="W9" s="171"/>
+      <c r="X9" s="172"/>
     </row>
     <row r="10" spans="2:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="12"/>
@@ -4705,12 +4705,12 @@
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
-      <c r="G10" s="172"/>
-      <c r="H10" s="173"/>
-      <c r="I10" s="174"/>
-      <c r="V10" s="172"/>
-      <c r="W10" s="173"/>
-      <c r="X10" s="174"/>
+      <c r="G10" s="170"/>
+      <c r="H10" s="171"/>
+      <c r="I10" s="172"/>
+      <c r="V10" s="170"/>
+      <c r="W10" s="171"/>
+      <c r="X10" s="172"/>
     </row>
     <row r="11" spans="2:24" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="12"/>
@@ -4718,19 +4718,19 @@
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
-      <c r="G11" s="175"/>
-      <c r="H11" s="176"/>
-      <c r="I11" s="177"/>
-      <c r="V11" s="175"/>
-      <c r="W11" s="176"/>
-      <c r="X11" s="177"/>
+      <c r="G11" s="173"/>
+      <c r="H11" s="174"/>
+      <c r="I11" s="175"/>
+      <c r="V11" s="173"/>
+      <c r="W11" s="174"/>
+      <c r="X11" s="175"/>
     </row>
     <row r="12" spans="2:24" ht="16" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="178"/>
-      <c r="C12" s="178"/>
-      <c r="D12" s="178"/>
-      <c r="E12" s="178"/>
-      <c r="F12" s="178"/>
+      <c r="B12" s="182"/>
+      <c r="C12" s="182"/>
+      <c r="D12" s="182"/>
+      <c r="E12" s="182"/>
+      <c r="F12" s="182"/>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B13" s="13"/>
@@ -4754,11 +4754,11 @@
       <c r="F15" s="12"/>
     </row>
     <row r="16" spans="2:24" ht="16" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="178"/>
-      <c r="C16" s="178"/>
-      <c r="D16" s="178"/>
-      <c r="E16" s="178"/>
-      <c r="F16" s="178"/>
+      <c r="B16" s="182"/>
+      <c r="C16" s="182"/>
+      <c r="D16" s="182"/>
+      <c r="E16" s="182"/>
+      <c r="F16" s="182"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="13"/>
@@ -4811,18 +4811,18 @@
     </row>
     <row r="35" spans="3:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="3:11" ht="14.5" x14ac:dyDescent="0.3">
-      <c r="D41" s="179" t="s">
+      <c r="D41" s="183" t="s">
         <v>71</v>
       </c>
-      <c r="E41" s="180"/>
-      <c r="F41" s="180"/>
-      <c r="G41" s="181"/>
-      <c r="H41" s="179" t="s">
+      <c r="E41" s="184"/>
+      <c r="F41" s="184"/>
+      <c r="G41" s="185"/>
+      <c r="H41" s="183" t="s">
         <v>72</v>
       </c>
-      <c r="I41" s="180"/>
-      <c r="J41" s="180"/>
-      <c r="K41" s="181"/>
+      <c r="I41" s="184"/>
+      <c r="J41" s="184"/>
+      <c r="K41" s="185"/>
     </row>
     <row r="42" spans="3:11" x14ac:dyDescent="0.3">
       <c r="D42" s="16" t="s">
@@ -5148,15 +5148,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="D41:G41"/>
+    <mergeCell ref="H41:K41"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="G8:I11"/>
     <mergeCell ref="G6:I6"/>
     <mergeCell ref="V6:X6"/>
     <mergeCell ref="V8:X11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="D41:G41"/>
-    <mergeCell ref="H41:K41"/>
   </mergeCells>
   <phoneticPr fontId="32"/>
   <conditionalFormatting sqref="F14">
@@ -5198,7 +5198,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:K94"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScalePageLayoutView="130" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7404,7 +7404,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="B1:H31"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScalePageLayoutView="130" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7919,7 +7919,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:L94"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScalePageLayoutView="130" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
@@ -10102,7 +10102,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B1:H31"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScalePageLayoutView="130" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>